<commit_message>
Redefine sweep values 10 points per range of possible capacities
</commit_message>
<xml_diff>
--- a/use_cases/LWR_FT_2023/data/HERON_data.xlsx
+++ b/use_cases/LWR_FT_2023/data/HERON_data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/LWR_FT_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEF6994-BF94-D64B-ADBF-DC2D3CE21483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3BA4B0-52EE-5E4B-83B2-487651442F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="2200" yWindow="1760" windowWidth="30720" windowHeight="17000" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
     <sheet name="Transfer_rates" sheetId="4" r:id="rId2"/>
     <sheet name="HTSE" sheetId="2" r:id="rId3"/>
     <sheet name="FT" sheetId="11" r:id="rId4"/>
-    <sheet name="Boundaries" sheetId="10" r:id="rId5"/>
+    <sheet name="Sweep values" sheetId="10" r:id="rId5"/>
     <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
     <sheet name="NPP_capacities" sheetId="12" r:id="rId7"/>
   </sheets>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="219">
   <si>
     <t>Source</t>
   </si>
@@ -337,27 +337,15 @@
     <t>Capacity negative when component is consuming a resource</t>
   </si>
   <si>
-    <t>Optimized components</t>
-  </si>
-  <si>
     <t>Lower</t>
   </si>
   <si>
     <t>Upper</t>
   </si>
   <si>
-    <t>kg-H2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Capacity  </t>
   </si>
   <si>
-    <t>htse</t>
-  </si>
-  <si>
-    <t>ft</t>
-  </si>
-  <si>
     <t>ft_elec_consumption</t>
   </si>
   <si>
@@ -370,9 +358,6 @@
     <t>naphtha_market</t>
   </si>
   <si>
-    <t>h2_storage</t>
-  </si>
-  <si>
     <t>Update from ANL August 2022</t>
   </si>
   <si>
@@ -460,18 +445,9 @@
     <t>kg-H2/MWh</t>
   </si>
   <si>
-    <t>npp</t>
-  </si>
-  <si>
     <t>elec_market</t>
   </si>
   <si>
-    <t>Elec to H2 rate (HTSE) = 25.13 kg-H2/MWh</t>
-  </si>
-  <si>
-    <t>100 kg initially stored, upper bound ~ 4h of storage for max capacity of FT</t>
-  </si>
-  <si>
     <t>Plant</t>
   </si>
   <si>
@@ -601,27 +577,6 @@
     <t>Federal corporate tax rate</t>
   </si>
   <si>
-    <t>Cooper</t>
-  </si>
-  <si>
-    <t>HTSE Lower (MWe)</t>
-  </si>
-  <si>
-    <t>HTSE Upper (MWe)</t>
-  </si>
-  <si>
-    <t>FT Lower (kg-H2)</t>
-  </si>
-  <si>
-    <t>FT Upper (kg-H2)</t>
-  </si>
-  <si>
-    <t>H2 storage Lower (kg-H2)</t>
-  </si>
-  <si>
-    <t>H2 storage Upper (kg-h2)</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -698,6 +653,51 @@
   </si>
   <si>
     <t>Depreciation schedule</t>
+  </si>
+  <si>
+    <t>Storage lower</t>
+  </si>
+  <si>
+    <t>10 so 0 storage</t>
+  </si>
+  <si>
+    <t>Storage upper</t>
+  </si>
+  <si>
+    <t>14 days worth of storage for the FT max capacity</t>
+  </si>
+  <si>
+    <t>HTSE Steps</t>
+  </si>
+  <si>
+    <t>FT Steps</t>
+  </si>
+  <si>
+    <t>Lower bound HTSE</t>
+  </si>
+  <si>
+    <t>100MW combined HTSE+FT power req</t>
+  </si>
+  <si>
+    <t>Higher bound HTSE</t>
+  </si>
+  <si>
+    <t>1000MW combined HTSE+FT power req</t>
+  </si>
+  <si>
+    <t>Constant Ft power req (MW)</t>
+  </si>
+  <si>
+    <t>HTSE (MWe)</t>
+  </si>
+  <si>
+    <t>FT (kg-H2)</t>
+  </si>
+  <si>
+    <t>H2 storage (kg-H2)</t>
+  </si>
+  <si>
+    <t>Hydrogen storage steps</t>
   </si>
 </sst>
 </file>
@@ -938,7 +938,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -974,6 +974,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2808,7 +2813,7 @@
         <v>25.125628140703519</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3024,7 +3029,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
@@ -3038,13 +3043,13 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M2" s="29" t="s">
         <v>26</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="O2" s="27" t="s">
         <v>27</v>
@@ -3058,65 +3063,65 @@
         <v>80</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="N3" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="O3" s="24">
         <v>257800644</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="N4" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="O4" s="24">
         <v>5156012.88</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>2019</v>
       </c>
       <c r="H5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="O5" s="24">
         <v>25780064.399999999</v>
       </c>
       <c r="P5" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="H6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I6">
         <v>100</v>
@@ -3129,18 +3134,18 @@
       </c>
       <c r="M6" s="30"/>
       <c r="N6" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="O6" s="24">
         <v>38670096.600000001</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <v>1.9E-2</v>
@@ -3159,21 +3164,21 @@
       </c>
       <c r="M7" s="30"/>
       <c r="N7" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="O7" s="24">
         <v>12251143</v>
       </c>
       <c r="P7" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
         <v>82</v>
@@ -3191,21 +3196,21 @@
       </c>
       <c r="M8" s="30"/>
       <c r="N8" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="O8" s="24">
         <v>38670096.600000001</v>
       </c>
       <c r="P8" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H9" t="s">
         <v>83</v>
@@ -3223,18 +3228,18 @@
         <v>0.3979400086720376</v>
       </c>
       <c r="M9" s="30" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="O9" s="24">
         <v>120527413.48</v>
       </c>
       <c r="P9" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I10">
         <f>LOG(I7)</f>
@@ -3249,126 +3254,126 @@
         <v>8.4682380044363352</v>
       </c>
       <c r="M10" s="30" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="N10" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="O10" s="24">
         <v>550360</v>
       </c>
       <c r="P10" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="M11" s="30" t="s">
         <v>81</v>
       </c>
       <c r="N11" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="O11" s="25">
         <v>378878417.48000002</v>
       </c>
       <c r="P11" s="14" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="M12" s="30" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="N12" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="O12" s="24">
         <v>9607972</v>
       </c>
       <c r="P12" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="N13" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="O13" s="24">
         <v>1921594.4</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B14">
         <v>10625</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="N14" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="O14" s="24">
         <v>7577568.3499999996</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B15">
         <f>155155000*(1+B7)</f>
         <v>158102945</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="M15" s="30" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="O15" s="24">
         <v>1049006</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -3380,13 +3385,13 @@
       </c>
       <c r="C16" s="1"/>
       <c r="M16" s="30" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="O16" s="25">
         <v>20156140.75</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -3400,35 +3405,35 @@
         <v>39</v>
       </c>
       <c r="M17" s="30" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="O17" s="24">
         <v>7085933</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="M18" s="30" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="O18" s="25">
         <v>7085933</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M19" s="31" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="N19" s="26" t="s">
         <v>4</v>
@@ -3442,7 +3447,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3450,7 +3455,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B21" s="20">
         <f>POWER(1+B7,4)*O18</f>
@@ -3464,7 +3469,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3472,14 +3477,14 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B25" s="20">
         <f>POWER(1+B7,4)*O16</f>
         <v>21732221.278510533</v>
       </c>
       <c r="C25" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3490,16 +3495,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
@@ -3508,421 +3514,1144 @@
     <col min="12" max="12" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>94</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" t="s">
-        <v>187</v>
-      </c>
-      <c r="H1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I1" t="s">
-        <v>189</v>
-      </c>
-      <c r="J1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K1" t="s">
-        <v>191</v>
-      </c>
-      <c r="L1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F2">
-        <v>1194</v>
-      </c>
-      <c r="G2">
-        <f>-F2+14.9</f>
-        <v>-1179.0999999999999</v>
-      </c>
-      <c r="H2">
-        <v>-100</v>
-      </c>
-      <c r="I2">
-        <f>G2*25.13</f>
-        <v>-29630.782999999996</v>
-      </c>
-      <c r="J2">
-        <f>H2*25.13</f>
-        <v>-2513</v>
-      </c>
-      <c r="K2">
-        <f>ABS(I2-25.13*H2)*2</f>
-        <v>54235.565999999992</v>
-      </c>
-      <c r="L2">
-        <f>ABS(I2)*4</f>
-        <v>118523.13199999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" t="s">
-        <v>156</v>
-      </c>
-      <c r="F3">
-        <v>894</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">-F3+14.9</f>
-        <v>-879.1</v>
-      </c>
-      <c r="H3">
-        <v>-100</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I8" si="1">G3*25.13</f>
-        <v>-22091.782999999999</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J8" si="2">H3*25.13</f>
-        <v>-2513</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K8" si="3">ABS(I3-25.13*H3)*2</f>
-        <v>39157.565999999999</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L8" si="4">ABS(I3)*4</f>
-        <v>88367.131999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4">
-        <v>1280</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>-1265.0999999999999</v>
-      </c>
-      <c r="H4">
-        <v>-100</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="1"/>
-        <v>-31791.962999999996</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="3"/>
-        <v>58557.925999999992</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="4"/>
-        <v>127167.85199999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="B5">
-        <v>1193</v>
+        <v>14.9</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
       </c>
-      <c r="E5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5">
-        <v>1138</v>
-      </c>
-      <c r="G5">
-        <f t="shared" si="0"/>
-        <v>-1123.0999999999999</v>
-      </c>
-      <c r="H5">
-        <v>-100</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="1"/>
-        <v>-28223.502999999997</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="3"/>
-        <v>51421.005999999994</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="4"/>
-        <v>112894.01199999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6">
-        <v>14.9</v>
+        <v>134</v>
+      </c>
+      <c r="B6" s="2">
+        <v>-9.9999999999999997E+199</v>
       </c>
       <c r="C6" t="s">
         <v>66</v>
       </c>
-      <c r="E6" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="2">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>214</v>
+      </c>
+      <c r="B15" s="34">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="H17" s="32"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19">
+        <v>1194</v>
+      </c>
+      <c r="C19">
+        <f>MAX(-B19+$B$15, -1000+$B$15)</f>
+        <v>-985.1</v>
+      </c>
+      <c r="D19" s="34">
+        <f>-100+$B$15</f>
+        <v>-85.1</v>
+      </c>
+      <c r="E19">
+        <f>C19*25.13</f>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="F19">
+        <f>D19*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+      <c r="G19">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>ABS(E19)*4</f>
+        <v>99022.251999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20">
+        <v>769</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:C23" si="0">MAX(-B20+$B$15, -1000+$B$15)</f>
+        <v>-754.1</v>
+      </c>
+      <c r="D20" s="34">
+        <f t="shared" ref="D20:D23" si="1">-100+$B$15</f>
+        <v>-85.1</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20" si="2">C20*25.13</f>
+        <v>-18950.532999999999</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20" si="3">D20*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+      <c r="G20">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20" si="4">ABS(E20)*4</f>
+        <v>75802.131999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21">
+        <v>894</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>-879.1</v>
+      </c>
+      <c r="D21" s="34">
+        <f t="shared" si="1"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E21">
+        <f>C21*25.13</f>
+        <v>-22091.782999999999</v>
+      </c>
+      <c r="F21">
+        <f>D21*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+      <c r="G21">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>ABS(E21)*4</f>
+        <v>88367.131999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22">
         <v>522</v>
       </c>
-      <c r="G6">
+      <c r="C22">
         <f t="shared" si="0"/>
         <v>-507.1</v>
       </c>
-      <c r="H6">
-        <v>-100</v>
-      </c>
-      <c r="I6">
+      <c r="D22" s="34">
         <f t="shared" si="1"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22" si="5">C22*25.13</f>
         <v>-12743.423000000001</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="3"/>
-        <v>20460.846000000001</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
+      <c r="F22">
+        <f t="shared" ref="F22" si="6">D22*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+      <c r="G22">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ref="H22" si="7">ABS(E22)*4</f>
         <v>50973.692000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7">
-        <v>769</v>
-      </c>
-      <c r="G7">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23">
+        <v>1280</v>
+      </c>
+      <c r="C23">
         <f t="shared" si="0"/>
+        <v>-985.1</v>
+      </c>
+      <c r="D23" s="34">
+        <f t="shared" si="1"/>
+        <v>-85.1</v>
+      </c>
+      <c r="E23">
+        <f>C23*25.13</f>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="F23">
+        <f>D23*25.13</f>
+        <v>-2138.5629999999996</v>
+      </c>
+      <c r="G23">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>ABS(E23)*24*14</f>
+        <v>8317869.1679999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+      <c r="J26">
+        <v>8</v>
+      </c>
+      <c r="K26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="33">
+        <f>$C19+B$26*ABS($C19-$D19)/9</f>
+        <v>-985.1</v>
+      </c>
+      <c r="C27" s="33">
+        <f t="shared" ref="C27:K27" si="8">$C19+C$26*ABS($C19-$D19)/9</f>
+        <v>-885.1</v>
+      </c>
+      <c r="D27" s="33">
+        <f t="shared" si="8"/>
+        <v>-785.1</v>
+      </c>
+      <c r="E27" s="33">
+        <f t="shared" si="8"/>
+        <v>-685.1</v>
+      </c>
+      <c r="F27" s="33">
+        <f t="shared" si="8"/>
+        <v>-585.1</v>
+      </c>
+      <c r="G27" s="33">
+        <f t="shared" si="8"/>
+        <v>-485.1</v>
+      </c>
+      <c r="H27" s="33">
+        <f t="shared" si="8"/>
+        <v>-385.1</v>
+      </c>
+      <c r="I27" s="33">
+        <f t="shared" si="8"/>
+        <v>-285.10000000000002</v>
+      </c>
+      <c r="J27" s="33">
+        <f t="shared" si="8"/>
+        <v>-185.10000000000002</v>
+      </c>
+      <c r="K27" s="33">
+        <f t="shared" si="8"/>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="33">
+        <f t="shared" ref="B28:K31" si="9">$C20+B$26*ABS($C20-$D20)/9</f>
         <v>-754.1</v>
       </c>
-      <c r="H7">
-        <v>-100</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
+      <c r="C28" s="33">
+        <f t="shared" si="9"/>
+        <v>-679.76666666666665</v>
+      </c>
+      <c r="D28" s="33">
+        <f t="shared" si="9"/>
+        <v>-605.43333333333339</v>
+      </c>
+      <c r="E28" s="33">
+        <f t="shared" si="9"/>
+        <v>-531.1</v>
+      </c>
+      <c r="F28" s="33">
+        <f t="shared" si="9"/>
+        <v>-456.76666666666671</v>
+      </c>
+      <c r="G28" s="33">
+        <f t="shared" si="9"/>
+        <v>-382.43333333333334</v>
+      </c>
+      <c r="H28" s="33">
+        <f t="shared" si="9"/>
+        <v>-308.10000000000002</v>
+      </c>
+      <c r="I28" s="33">
+        <f t="shared" si="9"/>
+        <v>-233.76666666666665</v>
+      </c>
+      <c r="J28" s="33">
+        <f t="shared" si="9"/>
+        <v>-159.43333333333339</v>
+      </c>
+      <c r="K28" s="33">
+        <f t="shared" si="9"/>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="33">
+        <f t="shared" si="9"/>
+        <v>-879.1</v>
+      </c>
+      <c r="C29" s="33">
+        <f t="shared" si="9"/>
+        <v>-790.87777777777774</v>
+      </c>
+      <c r="D29" s="33">
+        <f t="shared" si="9"/>
+        <v>-702.65555555555557</v>
+      </c>
+      <c r="E29" s="33">
+        <f t="shared" si="9"/>
+        <v>-614.43333333333339</v>
+      </c>
+      <c r="F29" s="33">
+        <f t="shared" si="9"/>
+        <v>-526.21111111111111</v>
+      </c>
+      <c r="G29" s="33">
+        <f t="shared" si="9"/>
+        <v>-437.98888888888894</v>
+      </c>
+      <c r="H29" s="33">
+        <f t="shared" si="9"/>
+        <v>-349.76666666666665</v>
+      </c>
+      <c r="I29" s="33">
+        <f t="shared" si="9"/>
+        <v>-261.54444444444448</v>
+      </c>
+      <c r="J29" s="33">
+        <f t="shared" si="9"/>
+        <v>-173.32222222222219</v>
+      </c>
+      <c r="K29" s="33">
+        <f t="shared" si="9"/>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>159</v>
+      </c>
+      <c r="B30" s="33">
+        <f t="shared" si="9"/>
+        <v>-507.1</v>
+      </c>
+      <c r="C30" s="33">
+        <f t="shared" si="9"/>
+        <v>-460.21111111111111</v>
+      </c>
+      <c r="D30" s="33">
+        <f t="shared" si="9"/>
+        <v>-413.32222222222225</v>
+      </c>
+      <c r="E30" s="33">
+        <f t="shared" si="9"/>
+        <v>-366.43333333333339</v>
+      </c>
+      <c r="F30" s="33">
+        <f t="shared" si="9"/>
+        <v>-319.54444444444448</v>
+      </c>
+      <c r="G30" s="33">
+        <f t="shared" si="9"/>
+        <v>-272.65555555555557</v>
+      </c>
+      <c r="H30" s="33">
+        <f t="shared" si="9"/>
+        <v>-225.76666666666671</v>
+      </c>
+      <c r="I30" s="33">
+        <f t="shared" si="9"/>
+        <v>-178.87777777777779</v>
+      </c>
+      <c r="J30" s="33">
+        <f t="shared" si="9"/>
+        <v>-131.98888888888894</v>
+      </c>
+      <c r="K30" s="33">
+        <f t="shared" si="9"/>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="33">
+        <f t="shared" si="9"/>
+        <v>-985.1</v>
+      </c>
+      <c r="C31" s="33">
+        <f t="shared" si="9"/>
+        <v>-885.1</v>
+      </c>
+      <c r="D31" s="33">
+        <f t="shared" si="9"/>
+        <v>-785.1</v>
+      </c>
+      <c r="E31" s="33">
+        <f t="shared" si="9"/>
+        <v>-685.1</v>
+      </c>
+      <c r="F31" s="33">
+        <f t="shared" si="9"/>
+        <v>-585.1</v>
+      </c>
+      <c r="G31" s="33">
+        <f t="shared" si="9"/>
+        <v>-485.1</v>
+      </c>
+      <c r="H31" s="33">
+        <f t="shared" si="9"/>
+        <v>-385.1</v>
+      </c>
+      <c r="I31" s="33">
+        <f t="shared" si="9"/>
+        <v>-285.10000000000002</v>
+      </c>
+      <c r="J31" s="33">
+        <f t="shared" si="9"/>
+        <v>-185.10000000000002</v>
+      </c>
+      <c r="K31" s="33">
+        <f t="shared" si="9"/>
+        <v>-85.100000000000023</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>6</v>
+      </c>
+      <c r="I34">
+        <v>7</v>
+      </c>
+      <c r="J34">
+        <v>8</v>
+      </c>
+      <c r="K34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="33">
+        <f>$E19+B$34*ABS($E19-$F19)/9</f>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="C35" s="33">
+        <f t="shared" ref="C35:K35" si="10">$E19+C$34*ABS($E19-$F19)/9</f>
+        <v>-22242.562999999998</v>
+      </c>
+      <c r="D35" s="33">
+        <f t="shared" si="10"/>
+        <v>-19729.562999999998</v>
+      </c>
+      <c r="E35" s="33">
+        <f t="shared" si="10"/>
+        <v>-17216.562999999998</v>
+      </c>
+      <c r="F35" s="33">
+        <f t="shared" si="10"/>
+        <v>-14703.562999999998</v>
+      </c>
+      <c r="G35" s="33">
+        <f t="shared" si="10"/>
+        <v>-12190.562999999998</v>
+      </c>
+      <c r="H35" s="33">
+        <f t="shared" si="10"/>
+        <v>-9677.5629999999983</v>
+      </c>
+      <c r="I35" s="33">
+        <f t="shared" si="10"/>
+        <v>-7164.5629999999983</v>
+      </c>
+      <c r="J35" s="33">
+        <f t="shared" si="10"/>
+        <v>-4651.5629999999983</v>
+      </c>
+      <c r="K35" s="33">
+        <f t="shared" si="10"/>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" s="33">
+        <f t="shared" ref="B36:K39" si="11">$E20+B$34*ABS($E20-$F20)/9</f>
         <v>-18950.532999999999</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="3"/>
-        <v>32875.065999999999</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
+      <c r="C36" s="33">
+        <f t="shared" si="11"/>
+        <v>-17082.536333333333</v>
+      </c>
+      <c r="D36" s="33">
+        <f t="shared" si="11"/>
+        <v>-15214.539666666666</v>
+      </c>
+      <c r="E36" s="33">
+        <f t="shared" si="11"/>
+        <v>-13346.542999999998</v>
+      </c>
+      <c r="F36" s="33">
+        <f t="shared" si="11"/>
+        <v>-11478.546333333332</v>
+      </c>
+      <c r="G36" s="33">
+        <f t="shared" si="11"/>
+        <v>-9610.5496666666659</v>
+      </c>
+      <c r="H36" s="33">
+        <f t="shared" si="11"/>
+        <v>-7742.5529999999981</v>
+      </c>
+      <c r="I36" s="33">
+        <f t="shared" si="11"/>
+        <v>-5874.5563333333321</v>
+      </c>
+      <c r="J36" s="33">
+        <f t="shared" si="11"/>
+        <v>-4006.5596666666643</v>
+      </c>
+      <c r="K36" s="33">
+        <f t="shared" si="11"/>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" s="33">
+        <f t="shared" si="11"/>
+        <v>-22091.782999999999</v>
+      </c>
+      <c r="C37" s="33">
+        <f t="shared" si="11"/>
+        <v>-19874.758555555556</v>
+      </c>
+      <c r="D37" s="33">
+        <f t="shared" si="11"/>
+        <v>-17657.734111111109</v>
+      </c>
+      <c r="E37" s="33">
+        <f t="shared" si="11"/>
+        <v>-15440.709666666666</v>
+      </c>
+      <c r="F37" s="33">
+        <f t="shared" si="11"/>
+        <v>-13223.685222222221</v>
+      </c>
+      <c r="G37" s="33">
+        <f t="shared" si="11"/>
+        <v>-11006.660777777777</v>
+      </c>
+      <c r="H37" s="33">
+        <f t="shared" si="11"/>
+        <v>-8789.636333333332</v>
+      </c>
+      <c r="I37" s="33">
+        <f t="shared" si="11"/>
+        <v>-6572.6118888888868</v>
+      </c>
+      <c r="J37" s="33">
+        <f t="shared" si="11"/>
+        <v>-4355.5874444444416</v>
+      </c>
+      <c r="K37" s="33">
+        <f t="shared" si="11"/>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" s="33">
+        <f t="shared" si="11"/>
+        <v>-12743.423000000001</v>
+      </c>
+      <c r="C38" s="33">
+        <f t="shared" si="11"/>
+        <v>-11565.105222222222</v>
+      </c>
+      <c r="D38" s="33">
+        <f t="shared" si="11"/>
+        <v>-10386.787444444446</v>
+      </c>
+      <c r="E38" s="33">
+        <f t="shared" si="11"/>
+        <v>-9208.4696666666678</v>
+      </c>
+      <c r="F38" s="33">
+        <f t="shared" si="11"/>
+        <v>-8030.1518888888895</v>
+      </c>
+      <c r="G38" s="33">
+        <f t="shared" si="11"/>
+        <v>-6851.8341111111113</v>
+      </c>
+      <c r="H38" s="33">
+        <f t="shared" si="11"/>
+        <v>-5673.5163333333339</v>
+      </c>
+      <c r="I38" s="33">
+        <f t="shared" si="11"/>
+        <v>-4495.1985555555566</v>
+      </c>
+      <c r="J38" s="33">
+        <f t="shared" si="11"/>
+        <v>-3316.8807777777783</v>
+      </c>
+      <c r="K38" s="33">
+        <f t="shared" si="11"/>
+        <v>-2138.5630000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="33">
+        <f t="shared" si="11"/>
+        <v>-24755.562999999998</v>
+      </c>
+      <c r="C39" s="33">
+        <f t="shared" si="11"/>
+        <v>-22242.562999999998</v>
+      </c>
+      <c r="D39" s="33">
+        <f t="shared" si="11"/>
+        <v>-19729.562999999998</v>
+      </c>
+      <c r="E39" s="33">
+        <f t="shared" si="11"/>
+        <v>-17216.562999999998</v>
+      </c>
+      <c r="F39" s="33">
+        <f t="shared" si="11"/>
+        <v>-14703.562999999998</v>
+      </c>
+      <c r="G39" s="33">
+        <f t="shared" si="11"/>
+        <v>-12190.562999999998</v>
+      </c>
+      <c r="H39" s="33">
+        <f t="shared" si="11"/>
+        <v>-9677.5629999999983</v>
+      </c>
+      <c r="I39" s="33">
+        <f t="shared" si="11"/>
+        <v>-7164.5629999999983</v>
+      </c>
+      <c r="J39" s="33">
+        <f t="shared" si="11"/>
+        <v>-4651.5629999999983</v>
+      </c>
+      <c r="K39" s="33">
+        <f t="shared" si="11"/>
+        <v>-2138.5629999999983</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <v>6</v>
+      </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+      <c r="J42">
+        <v>8</v>
+      </c>
+      <c r="K42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" s="33">
+        <f>B$42*ABS($G19-$H19)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="33">
+        <f t="shared" ref="C43:K43" si="12">C$42*ABS($G19-$H19)/9</f>
+        <v>11002.472444444444</v>
+      </c>
+      <c r="D43" s="33">
+        <f t="shared" si="12"/>
+        <v>22004.944888888887</v>
+      </c>
+      <c r="E43" s="33">
+        <f t="shared" si="12"/>
+        <v>33007.417333333331</v>
+      </c>
+      <c r="F43" s="33">
+        <f t="shared" si="12"/>
+        <v>44009.889777777775</v>
+      </c>
+      <c r="G43" s="33">
+        <f t="shared" si="12"/>
+        <v>55012.362222222218</v>
+      </c>
+      <c r="H43" s="33">
+        <f t="shared" si="12"/>
+        <v>66014.834666666662</v>
+      </c>
+      <c r="I43" s="33">
+        <f t="shared" si="12"/>
+        <v>77017.307111111106</v>
+      </c>
+      <c r="J43" s="33">
+        <f t="shared" si="12"/>
+        <v>88019.779555555549</v>
+      </c>
+      <c r="K43" s="33">
+        <f t="shared" si="12"/>
+        <v>99022.251999999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="33">
+        <f t="shared" ref="B44:K44" si="13">B$42*ABS($G20-$H20)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C44" s="33">
+        <f t="shared" si="13"/>
+        <v>8422.4591111111113</v>
+      </c>
+      <c r="D44" s="33">
+        <f t="shared" si="13"/>
+        <v>16844.918222222223</v>
+      </c>
+      <c r="E44" s="33">
+        <f t="shared" si="13"/>
+        <v>25267.377333333334</v>
+      </c>
+      <c r="F44" s="33">
+        <f t="shared" si="13"/>
+        <v>33689.836444444445</v>
+      </c>
+      <c r="G44" s="33">
+        <f t="shared" si="13"/>
+        <v>42112.295555555553</v>
+      </c>
+      <c r="H44" s="33">
+        <f t="shared" si="13"/>
+        <v>50534.754666666668</v>
+      </c>
+      <c r="I44" s="33">
+        <f t="shared" si="13"/>
+        <v>58957.213777777775</v>
+      </c>
+      <c r="J44" s="33">
+        <f t="shared" si="13"/>
+        <v>67379.67288888889</v>
+      </c>
+      <c r="K44" s="33">
+        <f t="shared" si="13"/>
         <v>75802.131999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" t="s">
-        <v>176</v>
-      </c>
-      <c r="F8">
-        <v>1314</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
-        <v>-1299.0999999999999</v>
-      </c>
-      <c r="H8">
-        <v>-100</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
-        <v>-32646.382999999998</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="2"/>
-        <v>-2513</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="3"/>
-        <v>60266.765999999996</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="4"/>
-        <v>130585.53199999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="2">
-        <v>-9.9999999999999997E+199</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>99</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B45" s="33">
+        <f t="shared" ref="B45:K45" si="14">B$42*ABS($G21-$H21)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="33">
+        <f t="shared" si="14"/>
+        <v>9818.5702222222226</v>
+      </c>
+      <c r="D45" s="33">
+        <f t="shared" si="14"/>
+        <v>19637.140444444445</v>
+      </c>
+      <c r="E45" s="33">
+        <f t="shared" si="14"/>
+        <v>29455.710666666666</v>
+      </c>
+      <c r="F45" s="33">
+        <f t="shared" si="14"/>
+        <v>39274.28088888889</v>
+      </c>
+      <c r="G45" s="33">
+        <f t="shared" si="14"/>
+        <v>49092.851111111107</v>
+      </c>
+      <c r="H45" s="33">
+        <f t="shared" si="14"/>
+        <v>58911.421333333332</v>
+      </c>
+      <c r="I45" s="33">
+        <f t="shared" si="14"/>
+        <v>68729.991555555549</v>
+      </c>
+      <c r="J45" s="33">
+        <f t="shared" si="14"/>
+        <v>78548.561777777781</v>
+      </c>
+      <c r="K45" s="33">
+        <f t="shared" si="14"/>
+        <v>88367.131999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>159</v>
+      </c>
+      <c r="B46" s="33">
+        <f t="shared" ref="B46:K46" si="15">B$42*ABS($G22-$H22)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C46" s="33">
+        <f t="shared" si="15"/>
+        <v>5663.7435555555558</v>
+      </c>
+      <c r="D46" s="33">
+        <f t="shared" si="15"/>
+        <v>11327.487111111112</v>
+      </c>
+      <c r="E46" s="33">
+        <f t="shared" si="15"/>
+        <v>16991.230666666666</v>
+      </c>
+      <c r="F46" s="33">
+        <f t="shared" si="15"/>
+        <v>22654.974222222223</v>
+      </c>
+      <c r="G46" s="33">
+        <f t="shared" si="15"/>
+        <v>28318.71777777778</v>
+      </c>
+      <c r="H46" s="33">
+        <f t="shared" si="15"/>
+        <v>33982.461333333333</v>
+      </c>
+      <c r="I46" s="33">
+        <f t="shared" si="15"/>
+        <v>39646.204888888897</v>
+      </c>
+      <c r="J46" s="33">
+        <f t="shared" si="15"/>
+        <v>45309.948444444446</v>
+      </c>
+      <c r="K46" s="33">
+        <f t="shared" si="15"/>
+        <v>50973.692000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B16">
-        <v>-1175</v>
-      </c>
-      <c r="C16">
-        <v>-100</v>
-      </c>
-      <c r="D16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17">
-        <f>B16*25.13</f>
-        <v>-29527.75</v>
-      </c>
-      <c r="C17">
-        <f>C16*25.13</f>
-        <v>-2513</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18">
-        <v>500</v>
-      </c>
-      <c r="C18">
-        <f>ABS(B17)*4</f>
-        <v>118111</v>
-      </c>
-      <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>186</v>
+      <c r="B47" s="33">
+        <f t="shared" ref="B47:K47" si="16">B$42*ABS($G23-$H23)/9</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="33">
+        <f t="shared" si="16"/>
+        <v>924207.68533333333</v>
+      </c>
+      <c r="D47" s="33">
+        <f t="shared" si="16"/>
+        <v>1848415.3706666667</v>
+      </c>
+      <c r="E47" s="33">
+        <f t="shared" si="16"/>
+        <v>2772623.0559999999</v>
+      </c>
+      <c r="F47" s="33">
+        <f t="shared" si="16"/>
+        <v>3696830.7413333333</v>
+      </c>
+      <c r="G47" s="33">
+        <f t="shared" si="16"/>
+        <v>4621038.4266666658</v>
+      </c>
+      <c r="H47" s="33">
+        <f t="shared" si="16"/>
+        <v>5545246.1119999997</v>
+      </c>
+      <c r="I47" s="33">
+        <f t="shared" si="16"/>
+        <v>6469453.7973333336</v>
+      </c>
+      <c r="J47" s="33">
+        <f t="shared" si="16"/>
+        <v>7393661.4826666666</v>
+      </c>
+      <c r="K47" s="33">
+        <f t="shared" si="16"/>
+        <v>8317869.1679999996</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:H17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4075,45 +4804,45 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -4122,13 +4851,13 @@
         <v>3645</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="H2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="I2" s="23">
         <v>9.5000000000000001E-2</v>
@@ -4140,13 +4869,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -4158,10 +4887,10 @@
         <v>894</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H3" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I3" s="23">
         <v>0</v>
@@ -4173,13 +4902,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -4191,10 +4920,10 @@
         <v>1280</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I4" s="23">
         <v>0</v>
@@ -4206,13 +4935,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B5" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -4221,13 +4950,13 @@
         <v>3411</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="H5" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="I5" s="23">
         <v>8.8400000000000006E-2</v>
@@ -4239,13 +4968,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B6" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -4254,13 +4983,13 @@
         <v>1677</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I6" s="23">
         <v>9.8000000000000004E-2</v>
@@ -4272,13 +5001,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -4290,10 +5019,10 @@
         <v>769</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="H7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="I7" s="23">
         <v>7.8100000000000003E-2</v>
@@ -4305,13 +5034,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -4320,13 +5049,13 @@
         <v>3990</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="I8" s="23">
         <v>4.9000000000000002E-2</v>
@@ -4341,7 +5070,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B10" s="22">
         <v>0.21</v>

</xml_diff>